<commit_message>
Removed redundant projects and made created NECB_PTool_Analysis.xlsx.   Added formatting for clarity and added BTAP outputs.
</commit_message>
<xml_diff>
--- a/projects/PTool_Full_Analysis.xlsx
+++ b/projects/PTool_Full_Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5250" windowWidth="20370" windowHeight="5265" tabRatio="469" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="5250" windowWidth="20370" windowHeight="5265" tabRatio="469" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -6349,8 +6349,36 @@
     <cellStyle name="Total" xfId="1817" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="1814" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6682,7 +6710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -7095,7 +7123,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12739,9 +12767,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13322,7 +13350,7 @@
       <c r="L19" s="34"/>
       <c r="M19" s="34"/>
     </row>
-    <row r="20" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
         <v>227</v>
       </c>

</xml_diff>